<commit_message>
close #156: Improve error message when parent and child have incompatible levels
</commit_message>
<xml_diff>
--- a/input_data/data_errors_09/descricao.xlsx
+++ b/input_data/data_errors_09/descricao.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="descricao" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="descricao" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -289,39 +289,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -397,17 +397,123 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Y866"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -574,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>22</v>
@@ -715,7 +821,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>36</v>

</xml_diff>